<commit_message>
cap nhat phan cong nhiem vu
</commit_message>
<xml_diff>
--- a/Semina/PhanCongNvu.xlsx
+++ b/Semina/PhanCongNvu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocLinh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocLinh\Desktop\PTTKTT\Thiet-Ke-Thuat-Toan\Semina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ADF18D-01D7-43ED-82C2-04CDD22A6BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFD0458-C7A1-4910-B9C3-CA8C7CE422DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Tổng hợp phát biểu ý kiến trong buổi ssemina</t>
+  </si>
+  <si>
+    <t>Giải quyết vài bài toán wecode</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -272,6 +275,26 @@
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -280,50 +303,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -333,6 +320,48 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
@@ -615,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,148 +657,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="14">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="23" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" ht="34.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="18">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="14" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="15"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="18">
         <v>3</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="14" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
         <v>4</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D16" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>